<commit_message>
Atualização da planilha de investimentos.
</commit_message>
<xml_diff>
--- a/investimentos.xlsx
+++ b/investimentos.xlsx
@@ -11,16 +11,17 @@
   </sheets>
   <definedNames>
     <definedName name="aporte">Plan1!$E$6</definedName>
-    <definedName name="caixinha">Plan1!$E$15</definedName>
-    <definedName name="fii">Plan1!$E$16</definedName>
-    <definedName name="ideal">Plan1!$E$8</definedName>
+    <definedName name="caixinha">Plan1!$E$16</definedName>
+    <definedName name="fii">Plan1!$E$17</definedName>
+    <definedName name="ideal">Plan1!$E$9</definedName>
     <definedName name="patrimonio">#REF!</definedName>
     <definedName name="qtd_anos">#REF!</definedName>
     <definedName name="rendimento_carteira">#REF!</definedName>
     <definedName name="salario">Plan1!$E$5</definedName>
     <definedName name="sugestao_investimento">#REF!</definedName>
     <definedName name="taxa_mensal">#REF!</definedName>
-    <definedName name="tesouro">Plan1!$E$14</definedName>
+    <definedName name="tempo">Plan1!$E$7</definedName>
+    <definedName name="tesouro">Plan1!$E$15</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -43,18 +44,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Salário</t>
   </si>
   <si>
-    <t>Correspondência</t>
-  </si>
-  <si>
     <t>FIIs</t>
-  </si>
-  <si>
-    <t>Ideal</t>
   </si>
   <si>
     <t>Possibilidade de investimento</t>
@@ -73,9 +68,6 @@
   </si>
   <si>
     <t>% rendimento mensal</t>
-  </si>
-  <si>
-    <t>Restante para ideal</t>
   </si>
   <si>
     <t>Patrimônio em 2 anos</t>
@@ -106,6 +98,21 @@
   </si>
   <si>
     <t>TIPOS DE INVESTIMENTO</t>
+  </si>
+  <si>
+    <t>Tempo de Investimento (em anos)</t>
+  </si>
+  <si>
+    <t>Patrimônio no tempo definido</t>
+  </si>
+  <si>
+    <t>% do salário</t>
+  </si>
+  <si>
+    <t>Valor ideal para investimento</t>
+  </si>
+  <si>
+    <t>Restante para atingir valor ideal</t>
   </si>
 </sst>
 </file>
@@ -212,7 +219,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -550,36 +557,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="dashed">
-        <color theme="2"/>
-      </left>
-      <right style="dashed">
-        <color theme="2"/>
-      </right>
-      <top style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="dashed">
-        <color theme="2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="dashed">
-        <color theme="2"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
-      </top>
-      <bottom style="dashed">
-        <color theme="2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -774,6 +751,86 @@
       </top>
       <bottom style="medium">
         <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="dashed">
+        <color theme="0"/>
+      </top>
+      <bottom style="dashed">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dashed">
+        <color theme="0"/>
+      </right>
+      <top style="dashed">
+        <color theme="0"/>
+      </top>
+      <bottom style="dashed">
+        <color theme="0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="dashed">
+        <color theme="2"/>
+      </top>
+      <bottom style="dashed">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="dashed">
+        <color theme="2"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color theme="2"/>
+      </left>
+      <right style="dashed">
+        <color theme="2"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dashed">
+        <color theme="2"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dashed">
+        <color theme="2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -786,32 +843,14 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="17" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -819,20 +858,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="4" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="4" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="4" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -851,11 +885,35 @@
     <xf numFmtId="9" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="3"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="37" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="30" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="31" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
@@ -875,27 +933,50 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="3"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="35" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="35" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="32" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="36" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="33" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="40" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="37" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="38" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="39" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="41" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="42" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="43" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="33" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -937,7 +1018,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Plan1!$C$21</c:f>
+              <c:f>Plan1!$C$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -951,7 +1032,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Plan1!$B$22:$B$25</c:f>
+              <c:f>Plan1!$B$24:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -972,7 +1053,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$D$22:$D$25</c:f>
+              <c:f>Plan1!$D$24:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>"R$"\ #,##0.00;[Red]\-"R$"\ #,##0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -997,7 +1078,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Plan1!$C$27</c:f>
+              <c:f>Plan1!$C$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1011,7 +1092,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Plan1!$B$22:$B$25</c:f>
+              <c:f>Plan1!$B$24:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1032,7 +1113,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$D$28:$D$31</c:f>
+              <c:f>Plan1!$D$31:$D$34</c:f>
               <c:numCache>
                 <c:formatCode>"R$"\ #,##0.00;[Red]\-"R$"\ #,##0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1057,7 +1138,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Plan1!$C$33</c:f>
+              <c:f>Plan1!$C$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1071,7 +1152,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Plan1!$B$22:$B$25</c:f>
+              <c:f>Plan1!$B$24:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1092,7 +1173,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Plan1!$D$34:$D$37</c:f>
+              <c:f>Plan1!$D$38:$D$41</c:f>
               <c:numCache>
                 <c:formatCode>"R$"\ #,##0.00;[Red]\-"R$"\ #,##0.00</c:formatCode>
                 <c:ptCount val="4"/>
@@ -1113,11 +1194,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="122810752"/>
-        <c:axId val="122813056"/>
+        <c:axId val="95291264"/>
+        <c:axId val="95292800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="122810752"/>
+        <c:axId val="95291264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,14 +1206,14 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122813056"/>
+        <c:crossAx val="95292800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122813056"/>
+        <c:axId val="95292800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1140,7 +1221,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122810752"/>
+        <c:crossAx val="95291264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1158,7 +1239,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000014" footer="0.31496062000000014"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000025" footer="0.31496062000000025"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1170,13 +1251,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>219075</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>38101</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1546,7 +1627,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1554,10 +1635,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:F37"/>
+  <dimension ref="B1:F41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1574,372 +1655,421 @@
     </row>
     <row r="3" spans="2:6" ht="15" thickBot="1"/>
     <row r="4" spans="2:6" ht="32.25" customHeight="1">
-      <c r="C4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="7"/>
+      <c r="C4" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
     </row>
     <row r="5" spans="2:6">
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="33"/>
-      <c r="E5" s="24">
+      <c r="D5" s="42"/>
+      <c r="E5" s="16">
         <v>3900</v>
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="C6" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="25">
+      <c r="C6" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="44"/>
+      <c r="E6" s="49">
         <v>1000</v>
       </c>
     </row>
     <row r="7" spans="2:6">
-      <c r="C7" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="35"/>
-      <c r="E7" s="26">
+      <c r="C7" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="46"/>
+      <c r="E7" s="50">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="C8" s="43" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="44"/>
+      <c r="E8" s="17">
         <f>aporte/salario</f>
         <v>0.25641025641025639</v>
       </c>
     </row>
-    <row r="8" spans="2:6">
-      <c r="C8" s="34" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="27">
+    <row r="9" spans="2:6">
+      <c r="C9" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="44"/>
+      <c r="E9" s="18">
         <f>salario*30%</f>
         <v>1170</v>
       </c>
     </row>
-    <row r="9" spans="2:6" ht="15" thickBot="1">
-      <c r="C9" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="37"/>
-      <c r="E9" s="28">
+    <row r="10" spans="2:6" ht="15" thickBot="1">
+      <c r="C10" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="48"/>
+      <c r="E10" s="19">
         <f>ideal-aporte</f>
         <v>170</v>
       </c>
     </row>
-    <row r="10" spans="2:6">
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="2:6" ht="15" thickBot="1">
+    <row r="11" spans="2:6">
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="2:6" ht="32.25" customHeight="1" thickBot="1">
-      <c r="C12" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="44"/>
-    </row>
-    <row r="13" spans="2:6" ht="15.75" thickBot="1">
-      <c r="C13" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6">
-      <c r="C14" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="29">
+    <row r="12" spans="2:6" ht="15" thickBot="1">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="2:6" ht="32.25" customHeight="1" thickBot="1">
+      <c r="C13" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="32"/>
+    </row>
+    <row r="14" spans="2:6" ht="15.75" thickBot="1">
+      <c r="C14" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="55"/>
+      <c r="E14" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6">
+      <c r="C15" s="37" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="38"/>
+      <c r="E15" s="20">
         <f>9.59%/12</f>
         <v>7.991666666666666E-3</v>
       </c>
-      <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="2:6">
-      <c r="C15" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="30">
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="2:6">
+      <c r="C16" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="34"/>
+      <c r="E16" s="21">
         <f>10.9%/12</f>
         <v>9.0833333333333339E-3</v>
       </c>
-      <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="2:6" ht="15" thickBot="1">
-      <c r="C16" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="37"/>
-      <c r="E16" s="31">
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="2:6" ht="15" thickBot="1">
+      <c r="C17" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="36"/>
+      <c r="E17" s="22">
         <f>12%/12</f>
         <v>0.01</v>
       </c>
-      <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="2:6">
-      <c r="D17" s="2"/>
-      <c r="E17" s="4"/>
       <c r="F17" s="4"/>
     </row>
-    <row r="18" spans="2:6" ht="15" thickBot="1">
+    <row r="18" spans="2:6">
       <c r="D18" s="2"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
     </row>
-    <row r="19" spans="2:6" ht="32.25" customHeight="1" thickBot="1">
-      <c r="C19" s="45" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="46"/>
-      <c r="E19" s="47" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" s="13" customFormat="1" ht="3.75" customHeight="1" thickBot="1">
-      <c r="B20" s="14"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-    </row>
-    <row r="21" spans="2:6" ht="15.75" thickBot="1">
-      <c r="C21" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="2:6">
-      <c r="B22" s="1">
-        <v>2</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="16">
-        <f>FV(tesouro,B22*12,aporte*-1)</f>
-        <v>26340.56765334267</v>
-      </c>
-      <c r="E22" s="17">
-        <f>D22*tesouro</f>
-        <v>210.50503649629681</v>
-      </c>
+    <row r="19" spans="2:6" ht="15" thickBot="1">
+      <c r="D19" s="2"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="2:6" ht="32.25" customHeight="1" thickBot="1">
+      <c r="C20" s="39" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="40"/>
+      <c r="E20" s="23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" s="7" customFormat="1" ht="3.75" customHeight="1" thickBot="1">
+      <c r="B21" s="8"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="22" spans="2:6" ht="15.75" thickBot="1">
+      <c r="C22" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="25"/>
+      <c r="E22" s="26"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="1">
-        <v>5</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="19">
-        <f>FV(tesouro,B23*12,aporte*-1)</f>
-        <v>76603.674875050565</v>
-      </c>
-      <c r="E23" s="20">
+      <c r="C23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="52">
+        <f>FV(tesouro,tempo*12,aporte*-1)</f>
+        <v>399208.63525201735</v>
+      </c>
+      <c r="E23" s="53">
         <f>D23*tesouro</f>
-        <v>612.19103504311238</v>
+        <v>3190.3423433890384</v>
       </c>
     </row>
     <row r="24" spans="2:6">
       <c r="B24" s="1">
+        <v>2</v>
+      </c>
+      <c r="C24" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="52">
+        <f>FV(tesouro,B24*12,aporte*-1)</f>
+        <v>26340.56765334267</v>
+      </c>
+      <c r="E24" s="53">
+        <f>D24*tesouro</f>
+        <v>210.50503649629681</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6">
+      <c r="B25" s="1">
+        <v>5</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="11">
+        <f>FV(tesouro,B25*12,aporte*-1)</f>
+        <v>76603.674875050565</v>
+      </c>
+      <c r="E25" s="12">
+        <f>D25*tesouro</f>
+        <v>612.19103504311238</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6">
+      <c r="B26" s="1">
         <v>10</v>
       </c>
-      <c r="C24" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="19">
-        <f>FV(tesouro,B24*12,aporte*-1)</f>
+      <c r="C26" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="11">
+        <f>FV(tesouro,B26*12,aporte*-1)</f>
         <v>200103.43275996446</v>
       </c>
-      <c r="E24" s="20">
-        <f>D24*tesouro</f>
+      <c r="E26" s="12">
+        <f>D26*tesouro</f>
         <v>1599.1599334733826</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="15" thickBot="1">
-      <c r="B25" s="1">
+    <row r="27" spans="2:6" ht="15" thickBot="1">
+      <c r="B27" s="1">
         <v>20</v>
       </c>
-      <c r="C25" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="22">
-        <f>FV(tesouro,B25*12,aporte*-1)</f>
+      <c r="C27" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="14">
+        <f>FV(tesouro,B27*12,aporte*-1)</f>
         <v>720204.25774014881</v>
       </c>
-      <c r="E25" s="23">
-        <f>D25*tesouro</f>
+      <c r="E27" s="15">
+        <f>D27*tesouro</f>
         <v>5755.6323597733553</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="4.5" customHeight="1" thickBot="1"/>
-    <row r="27" spans="2:6" ht="15.75" thickBot="1">
-      <c r="C27" s="9" t="s">
+    <row r="28" spans="2:6" ht="4.5" customHeight="1" thickBot="1"/>
+    <row r="29" spans="2:6" ht="15.75" thickBot="1">
+      <c r="C29" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="25"/>
+      <c r="E29" s="26"/>
+    </row>
+    <row r="30" spans="2:6">
+      <c r="C30" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D27" s="10"/>
-      <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="2:6">
-      <c r="B28" s="1">
+      <c r="D30" s="52">
+        <f>FV(caixinha,tempo*12,aporte*-1)</f>
+        <v>450466.46288975165</v>
+      </c>
+      <c r="E30" s="53">
+        <f>D30*caixinha</f>
+        <v>4091.7370379152444</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6">
+      <c r="B31" s="1">
         <v>2</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C31" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="52">
+        <f>FV(caixinha,B31*12,aporte*-1)</f>
+        <v>26682.255446927989</v>
+      </c>
+      <c r="E31" s="53">
+        <f>D31*caixinha</f>
+        <v>242.36382030959592</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6">
+      <c r="B32" s="1">
+        <v>5</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="11">
+        <f>FV(caixinha,B32*12,aporte*-1)</f>
+        <v>79306.844879213546</v>
+      </c>
+      <c r="E32" s="12">
+        <f>D32*caixinha</f>
+        <v>720.37050765285642</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5">
+      <c r="B33" s="1">
+        <v>10</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="11">
+        <f>FV(caixinha,B33*12,aporte*-1)</f>
+        <v>215744.00186441257</v>
+      </c>
+      <c r="E33" s="12">
+        <f>D33*caixinha</f>
+        <v>1959.6746836017476</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="15" thickBot="1">
+      <c r="B34" s="1">
+        <v>20</v>
+      </c>
+      <c r="C34" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="16">
-        <f>FV(caixinha,B28*12,aporte*-1)</f>
-        <v>26682.255446927989</v>
-      </c>
-      <c r="E28" s="17">
-        <f>D28*caixinha</f>
-        <v>242.36382030959592</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6">
-      <c r="B29" s="1">
+      <c r="D34" s="14">
+        <f>FV(caixinha,B34*12,aporte*-1)</f>
+        <v>854276.06232144241</v>
+      </c>
+      <c r="E34" s="15">
+        <f>D34*caixinha</f>
+        <v>7759.6742327531019</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="3.75" customHeight="1" thickBot="1"/>
+    <row r="36" spans="2:5" ht="15.75" thickBot="1">
+      <c r="C36" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="25"/>
+      <c r="E36" s="26"/>
+    </row>
+    <row r="37" spans="2:5">
+      <c r="C37" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="52">
+        <f>FV(fii,tempo*12,aporte*-1)</f>
+        <v>499580.19753561798</v>
+      </c>
+      <c r="E37" s="53">
+        <f>D37*fii</f>
+        <v>4995.8019753561803</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="1">
+        <v>2</v>
+      </c>
+      <c r="C38" s="51" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="52">
+        <f>FV(fii,B38*12,aporte*-1)</f>
+        <v>26973.464853191497</v>
+      </c>
+      <c r="E38" s="53">
+        <f>D38*fii</f>
+        <v>269.73464853191496</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5">
+      <c r="B39" s="1">
         <v>5</v>
       </c>
-      <c r="C29" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="19">
-        <f>FV(caixinha,B29*12,aporte*-1)</f>
-        <v>79306.844879213546</v>
-      </c>
-      <c r="E29" s="20">
-        <f>D29*caixinha</f>
-        <v>720.37050765285642</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6">
-      <c r="B30" s="1">
+      <c r="C39" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="11">
+        <f>FV(fii,B39*12,aporte*-1)</f>
+        <v>81669.669856409135</v>
+      </c>
+      <c r="E39" s="12">
+        <f>D39*fii</f>
+        <v>816.69669856409132</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="B40" s="1">
         <v>10</v>
       </c>
-      <c r="C30" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="19">
-        <f>FV(caixinha,B30*12,aporte*-1)</f>
-        <v>215744.00186441257</v>
-      </c>
-      <c r="E30" s="20">
-        <f>D30*caixinha</f>
-        <v>1959.6746836017476</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" ht="15" thickBot="1">
-      <c r="B31" s="1">
+      <c r="C40" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="11">
+        <f>FV(fii,B40*12,aporte*-1)</f>
+        <v>230038.68945736697</v>
+      </c>
+      <c r="E40" s="12">
+        <f>D40*fii</f>
+        <v>2300.3868945736699</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="15" thickBot="1">
+      <c r="B41" s="1">
         <v>20</v>
       </c>
-      <c r="C31" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="22">
-        <f>FV(caixinha,B31*12,aporte*-1)</f>
-        <v>854276.06232144241</v>
-      </c>
-      <c r="E31" s="23">
-        <f>D31*caixinha</f>
-        <v>7759.6742327531019</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" ht="3.75" customHeight="1" thickBot="1"/>
-    <row r="33" spans="2:5" ht="15.75" thickBot="1">
-      <c r="C33" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D33" s="10"/>
-      <c r="E33" s="11"/>
-    </row>
-    <row r="34" spans="2:5">
-      <c r="B34" s="1">
-        <v>2</v>
-      </c>
-      <c r="C34" s="15" t="s">
+      <c r="C41" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="16">
-        <f>FV(fii,B34*12,aporte*-1)</f>
-        <v>26973.464853191497</v>
-      </c>
-      <c r="E34" s="17">
-        <f>D34*fii</f>
-        <v>269.73464853191496</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5">
-      <c r="B35" s="1">
-        <v>5</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="19">
-        <f>FV(fii,B35*12,aporte*-1)</f>
-        <v>81669.669856409135</v>
-      </c>
-      <c r="E35" s="20">
-        <f>D35*fii</f>
-        <v>816.69669856409132</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5">
-      <c r="B36" s="1">
-        <v>10</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D36" s="19">
-        <f>FV(fii,B36*12,aporte*-1)</f>
-        <v>230038.68945736697</v>
-      </c>
-      <c r="E36" s="20">
-        <f>D36*fii</f>
-        <v>2300.3868945736699</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="15" thickBot="1">
-      <c r="B37" s="1">
-        <v>20</v>
-      </c>
-      <c r="C37" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="22">
-        <f>FV(fii,B37*12,aporte*-1)</f>
+      <c r="D41" s="14">
+        <f>FV(fii,B41*12,aporte*-1)</f>
         <v>989255.36538736301</v>
       </c>
-      <c r="E37" s="23">
-        <f>D37*fii</f>
+      <c r="E41" s="15">
+        <f>D41*fii</f>
         <v>9892.5536538736305</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="C33:E33"/>
+  <mergeCells count="16">
+    <mergeCell ref="C36:E36"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C10:D10"/>
     <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="C27:E27"/>
     <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C29:E29"/>
     <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C7:D7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1948,12 +2078,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851b35d3-0456-4d6a-bc2f-da927e91d158">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="19483571-f922-4e8e-9c1c-26f0a2252132" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2212,20 +2344,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="851b35d3-0456-4d6a-bc2f-da927e91d158">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="19483571-f922-4e8e-9c1c-26f0a2252132" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C32110DE-3D77-470C-9CED-65521C30E3F6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54D0D6DD-E6DB-45C8-8F90-E314C090C085}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
+    <ds:schemaRef ds:uri="19483571-f922-4e8e-9c1c-26f0a2252132"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2250,12 +2383,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54D0D6DD-E6DB-45C8-8F90-E314C090C085}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C32110DE-3D77-470C-9CED-65521C30E3F6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="851b35d3-0456-4d6a-bc2f-da927e91d158"/>
-    <ds:schemaRef ds:uri="19483571-f922-4e8e-9c1c-26f0a2252132"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>